<commit_message>
HomeOffice report uses Excel template
This template now loads a report template from the database along with
the header mappings and sheet to update.
A validator is also added to has all the required info to generate
report successfully
</commit_message>
<xml_diff>
--- a/spec/fixtures/test_homeoffice_template.xlsx
+++ b/spec/fixtures/test_homeoffice_template.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Landing" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Data" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="TestData" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Data" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t xml:space="preserve">This is a test file</t>
   </si>
@@ -33,6 +34,57 @@
   </si>
   <si>
     <t xml:space="preserve">bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nationality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place of Birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passport Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Insurance Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID (Mandatory)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Name/ Organisation Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dummy 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dummy 2</t>
   </si>
 </sst>
 </file>
@@ -135,11 +187,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B:B A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -162,13 +214,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B:B A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -179,6 +231,118 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>